<commit_message>
Adding HTML version of book description. Changing figure label to white.
</commit_message>
<xml_diff>
--- a/extras/ChartsStandardizedVocabularies.xlsx
+++ b/extras/ChartsStandardizedVocabularies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mschuemi\Git\TheBookOfOhdsi\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6548BF4B-B155-4D2D-93B3-233C524D9E7D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1C007E-20A9-4259-8022-0C0B3578A569}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{CBA506A4-9AB1-47DE-B51B-B0412BA82668}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{CBA506A4-9AB1-47DE-B51B-B0412BA82668}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -143,6 +143,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA7E8FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -247,6 +252,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-4577-4EA4-88C6-1D446FFFF7DE}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -330,6 +340,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-4577-4EA4-88C6-1D446FFFF7DE}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -368,6 +383,45 @@
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-F5F7-4F56-A72B-248EB1F1C273}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-4577-4EA4-88C6-1D446FFFF7DE}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -681,6 +735,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B766-4548-82BE-78DD3618493C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -696,6 +755,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B766-4548-82BE-78DD3618493C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -711,6 +775,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B766-4548-82BE-78DD3618493C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -726,6 +795,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-B766-4548-82BE-78DD3618493C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -741,6 +815,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-B766-4548-82BE-78DD3618493C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -756,6 +835,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-B766-4548-82BE-78DD3618493C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -773,6 +857,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-B766-4548-82BE-78DD3618493C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -790,6 +879,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-B766-4548-82BE-78DD3618493C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -807,6 +901,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-B766-4548-82BE-78DD3618493C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2505,8 +2604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D76A5E5-8650-4997-B337-3A23CF1C7BC7}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2585,7 +2684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF65BE6-7497-48FE-A8F5-E75DE0DB4F26}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>

</xml_diff>